<commit_message>
Changes in titles HTML
</commit_message>
<xml_diff>
--- a/respuestas/registro/registro.xlsx
+++ b/respuestas/registro/registro.xlsx
@@ -642,10 +642,110 @@
       <c r="A4" t="n">
         <v>3</v>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>asda</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>sdasdasd</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>asdasdasd</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2021-03-10</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Casado</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>asda</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>sdasdasd</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>asdasdasd</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2021-03-10</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Casado</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
       </c>
     </row>
     <row r="6">

</xml_diff>